<commit_message>
Added new figures for scaling
</commit_message>
<xml_diff>
--- a/latex/performance_content/scaling/ItascaScaling.xlsx
+++ b/latex/performance_content/scaling/ItascaScaling.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="43540" windowHeight="27320" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28420" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Strong 4.096M nodes" sheetId="1" r:id="rId1"/>
@@ -290,7 +290,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="454">
+  <cellStyleXfs count="460">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -745,6 +745,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -762,7 +768,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="41" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="454">
+  <cellStyles count="460">
     <cellStyle name="Comma" xfId="40" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -997,6 +1003,9 @@
     <cellStyle name="Followed Hyperlink" xfId="449" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="451" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="453" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="455" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="457" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="459" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1215,6 +1224,9 @@
     <cellStyle name="Hyperlink" xfId="448" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="450" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="452" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="454" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="456" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="458" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="41" builtinId="5"/>
   </cellStyles>
@@ -1260,7 +1272,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1644,11 +1655,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1788112184"/>
-        <c:axId val="1788117736"/>
+        <c:axId val="2070879304"/>
+        <c:axId val="2070882600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1788112184"/>
+        <c:axId val="2070879304"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1671,19 +1682,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788117736"/>
+        <c:crossAx val="2070882600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1788117736"/>
+        <c:axId val="2070882600"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1712,14 +1722,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788112184"/>
+        <c:crossAx val="2070879304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1730,7 +1739,6 @@
         <c:idx val="3"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2165,11 +2173,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1788391208"/>
-        <c:axId val="1788396760"/>
+        <c:axId val="2087454328"/>
+        <c:axId val="2087459672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1788391208"/>
+        <c:axId val="2087454328"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2198,12 +2206,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788396760"/>
+        <c:crossAx val="2087459672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1788396760"/>
+        <c:axId val="2087459672"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2238,7 +2246,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788391208"/>
+        <c:crossAx val="2087454328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2721,11 +2729,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1788527240"/>
-        <c:axId val="1788532792"/>
+        <c:axId val="2087520408"/>
+        <c:axId val="2087525944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1788527240"/>
+        <c:axId val="2087520408"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2754,12 +2762,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788532792"/>
+        <c:crossAx val="2087525944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1788532792"/>
+        <c:axId val="2087525944"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2789,7 +2797,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788527240"/>
+        <c:crossAx val="2087520408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3168,11 +3176,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121946296"/>
-        <c:axId val="2121545096"/>
+        <c:axId val="2087563256"/>
+        <c:axId val="2087568728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121946296"/>
+        <c:axId val="2087563256"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -3201,12 +3209,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121545096"/>
+        <c:crossAx val="2087568728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121545096"/>
+        <c:axId val="2087568728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3235,7 +3243,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121946296"/>
+        <c:crossAx val="2087563256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3315,7 +3323,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3590,11 +3597,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1788437176"/>
-        <c:axId val="1788442648"/>
+        <c:axId val="2087606136"/>
+        <c:axId val="2087611624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1788437176"/>
+        <c:axId val="2087606136"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -3617,19 +3624,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788442648"/>
+        <c:crossAx val="2087611624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1788442648"/>
+        <c:axId val="2087611624"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -3658,21 +3664,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788437176"/>
+        <c:crossAx val="2087606136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3729,7 +3733,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4134,11 +4137,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1788572584"/>
-        <c:axId val="1788578136"/>
+        <c:axId val="2112096344"/>
+        <c:axId val="2112101912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1788572584"/>
+        <c:axId val="2112096344"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -4161,19 +4164,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788578136"/>
+        <c:crossAx val="2112101912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1788578136"/>
+        <c:axId val="2112101912"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -4202,14 +4204,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788572584"/>
+        <c:crossAx val="2112096344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4220,7 +4221,6 @@
         <c:idx val="1"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4277,7 +4277,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4585,11 +4584,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2065069464"/>
-        <c:axId val="2065074936"/>
+        <c:axId val="2112146888"/>
+        <c:axId val="2112152376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2065069464"/>
+        <c:axId val="2112146888"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -4612,19 +4611,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065074936"/>
+        <c:crossAx val="2112152376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2065074936"/>
+        <c:axId val="2112152376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4647,14 +4645,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065069464"/>
+        <c:crossAx val="2112146888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4667,7 +4664,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4719,7 +4715,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5336,11 +5331,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2065128936"/>
-        <c:axId val="2065134568"/>
+        <c:axId val="2112206088"/>
+        <c:axId val="2112211704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2065128936"/>
+        <c:axId val="2112206088"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5363,19 +5358,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065134568"/>
+        <c:crossAx val="2112211704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2065134568"/>
+        <c:axId val="2112211704"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5404,14 +5398,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065128936"/>
+        <c:crossAx val="2112206088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5424,7 +5417,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5476,7 +5468,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5775,11 +5766,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2065169416"/>
-        <c:axId val="2065174920"/>
+        <c:axId val="2112246056"/>
+        <c:axId val="2112251576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2065169416"/>
+        <c:axId val="2112246056"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5802,19 +5793,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065174920"/>
+        <c:crossAx val="2112251576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2065174920"/>
+        <c:axId val="2112251576"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5843,21 +5833,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065169416"/>
+        <c:crossAx val="2112246056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5909,7 +5897,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6326,11 +6313,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2073656264"/>
-        <c:axId val="-2073662280"/>
+        <c:axId val="2112295832"/>
+        <c:axId val="2112301400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2073656264"/>
+        <c:axId val="2112295832"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -6353,19 +6340,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073662280"/>
+        <c:crossAx val="2112301400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2073662280"/>
+        <c:axId val="2112301400"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -6389,14 +6375,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073656264"/>
+        <c:crossAx val="2112295832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6409,7 +6394,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6462,7 +6446,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6779,11 +6762,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2073687992"/>
-        <c:axId val="-2073685352"/>
+        <c:axId val="2112338872"/>
+        <c:axId val="2112344392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2073687992"/>
+        <c:axId val="2112338872"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -6806,19 +6789,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073685352"/>
+        <c:crossAx val="2112344392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2073685352"/>
+        <c:axId val="2112344392"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -6847,14 +6829,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073687992"/>
+        <c:crossAx val="2112338872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6867,7 +6848,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6924,7 +6904,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7411,11 +7390,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1788167592"/>
-        <c:axId val="1788173288"/>
+        <c:axId val="2069955496"/>
+        <c:axId val="2069949784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1788167592"/>
+        <c:axId val="2069955496"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -7438,19 +7417,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788173288"/>
+        <c:crossAx val="2069949784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1788173288"/>
+        <c:axId val="2069949784"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -7474,14 +7452,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788167592"/>
+        <c:crossAx val="2069955496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7492,7 +7469,6 @@
         <c:idx val="0"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7544,7 +7520,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7861,11 +7836,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2078647480"/>
-        <c:axId val="-2043863352"/>
+        <c:axId val="2112383928"/>
+        <c:axId val="2112389432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2078647480"/>
+        <c:axId val="2112383928"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -7888,19 +7863,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2043863352"/>
+        <c:crossAx val="2112389432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2043863352"/>
+        <c:axId val="2112389432"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -7929,14 +7903,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2078647480"/>
+        <c:crossAx val="2112383928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7949,7 +7922,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8419,11 +8391,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2070434920"/>
-        <c:axId val="2070440504"/>
+        <c:axId val="2083083176"/>
+        <c:axId val="2083088760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2070434920"/>
+        <c:axId val="2083083176"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -8453,12 +8425,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2070440504"/>
+        <c:crossAx val="2083088760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2070440504"/>
+        <c:axId val="2083088760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8492,7 +8464,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2070434920"/>
+        <c:crossAx val="2083083176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8969,11 +8941,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2070500392"/>
-        <c:axId val="2070505976"/>
+        <c:axId val="2083132008"/>
+        <c:axId val="2083137592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2070500392"/>
+        <c:axId val="2083132008"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -9003,12 +8975,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2070505976"/>
+        <c:crossAx val="2083137592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2070505976"/>
+        <c:axId val="2083137592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9042,7 +9014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2070500392"/>
+        <c:crossAx val="2083132008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9487,11 +9459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2070545336"/>
-        <c:axId val="2070550920"/>
+        <c:axId val="2083177144"/>
+        <c:axId val="2083182728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2070545336"/>
+        <c:axId val="2083177144"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -9521,12 +9493,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2070550920"/>
+        <c:crossAx val="2083182728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2070550920"/>
+        <c:axId val="2083182728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9560,7 +9532,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2070545336"/>
+        <c:crossAx val="2083177144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9921,11 +9893,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2070586952"/>
-        <c:axId val="2070592456"/>
+        <c:axId val="2122590008"/>
+        <c:axId val="2122586440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2070586952"/>
+        <c:axId val="2122590008"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -9955,12 +9927,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2070592456"/>
+        <c:crossAx val="2122586440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2070592456"/>
+        <c:axId val="2122586440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9994,7 +9966,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2070586952"/>
+        <c:crossAx val="2122590008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10388,11 +10360,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2073677240"/>
-        <c:axId val="-2073674600"/>
+        <c:axId val="2112452680"/>
+        <c:axId val="2112458152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2073677240"/>
+        <c:axId val="2112452680"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -10422,12 +10394,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073674600"/>
+        <c:crossAx val="2112458152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2073674600"/>
+        <c:axId val="2112458152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10461,7 +10433,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073677240"/>
+        <c:crossAx val="2112452680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10817,11 +10789,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2073712952"/>
-        <c:axId val="-2073723512"/>
+        <c:axId val="2112494424"/>
+        <c:axId val="2112499944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2073712952"/>
+        <c:axId val="2112494424"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -10851,12 +10823,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073723512"/>
+        <c:crossAx val="2112499944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2073723512"/>
+        <c:axId val="2112499944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10890,7 +10862,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073712952"/>
+        <c:crossAx val="2112494424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11761,11 +11733,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2073755816"/>
-        <c:axId val="-2073762344"/>
+        <c:axId val="2112563768"/>
+        <c:axId val="2112569304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2073755816"/>
+        <c:axId val="2112563768"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -11795,12 +11767,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073762344"/>
+        <c:crossAx val="2112569304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2073762344"/>
+        <c:axId val="2112569304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11834,7 +11806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073755816"/>
+        <c:crossAx val="2112563768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12308,11 +12280,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2021597464"/>
-        <c:axId val="-2129372024"/>
+        <c:axId val="2112606472"/>
+        <c:axId val="2112612056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2021597464"/>
+        <c:axId val="2112606472"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -12342,12 +12314,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129372024"/>
+        <c:crossAx val="2112612056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129372024"/>
+        <c:axId val="2112612056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0"/>
@@ -12382,7 +12354,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021597464"/>
+        <c:crossAx val="2112606472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12439,7 +12411,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -12956,11 +12927,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2073815752"/>
-        <c:axId val="-2073823048"/>
+        <c:axId val="2112693496"/>
+        <c:axId val="2112699464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2073815752"/>
+        <c:axId val="2112693496"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -12988,19 +12959,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073823048"/>
+        <c:crossAx val="2112699464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2073823048"/>
+        <c:axId val="2112699464"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -13024,21 +12994,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073815752"/>
+        <c:crossAx val="2112693496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13095,7 +13063,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -13412,11 +13379,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1788211032"/>
-        <c:axId val="1788216504"/>
+        <c:axId val="2087293880"/>
+        <c:axId val="2087299368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1788211032"/>
+        <c:axId val="2087293880"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -13439,19 +13406,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788216504"/>
+        <c:crossAx val="2087299368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1788216504"/>
+        <c:axId val="2087299368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13474,14 +13440,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788211032"/>
+        <c:crossAx val="2087293880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13494,7 +13459,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13544,7 +13508,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -13971,11 +13934,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2073848296"/>
-        <c:axId val="-2073853896"/>
+        <c:axId val="2112742168"/>
+        <c:axId val="2112747992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2073848296"/>
+        <c:axId val="2112742168"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -14003,19 +13966,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073853896"/>
+        <c:crossAx val="2112747992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2073853896"/>
+        <c:axId val="2112747992"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -14039,21 +14001,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073848296"/>
+        <c:crossAx val="2112742168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14103,7 +14063,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -14620,11 +14579,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2073886392"/>
-        <c:axId val="-2073890616"/>
+        <c:axId val="2112794440"/>
+        <c:axId val="2112800408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2073886392"/>
+        <c:axId val="2112794440"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -14652,19 +14611,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073890616"/>
+        <c:crossAx val="2112800408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2073890616"/>
+        <c:axId val="2112800408"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -14688,21 +14646,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073886392"/>
+        <c:crossAx val="2112794440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14747,7 +14703,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -15164,11 +15119,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2073915736"/>
-        <c:axId val="-2073922008"/>
+        <c:axId val="2112837160"/>
+        <c:axId val="2083025832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2073915736"/>
+        <c:axId val="2112837160"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -15176,19 +15131,18 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073922008"/>
+        <c:crossAx val="2083025832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2073922008"/>
+        <c:axId val="2083025832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -15197,21 +15151,19 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073915736"/>
+        <c:crossAx val="2112837160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15475,11 +15427,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2073943720"/>
-        <c:axId val="-2073950648"/>
+        <c:axId val="2083260872"/>
+        <c:axId val="2083266408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2073943720"/>
+        <c:axId val="2083260872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15508,7 +15460,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073950648"/>
+        <c:crossAx val="2083266408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15516,7 +15468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2073950648"/>
+        <c:axId val="2083266408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15546,7 +15498,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073943720"/>
+        <c:crossAx val="2083260872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -15601,7 +15553,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -15718,11 +15669,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2073979736"/>
-        <c:axId val="-2073984072"/>
+        <c:axId val="2083301048"/>
+        <c:axId val="2083306808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2073979736"/>
+        <c:axId val="2083301048"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -15750,19 +15701,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073984072"/>
+        <c:crossAx val="2083306808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2073984072"/>
+        <c:axId val="2083306808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15785,21 +15735,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073979736"/>
+        <c:crossAx val="2083301048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15849,7 +15797,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -16169,11 +16116,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2074017096"/>
-        <c:axId val="-2074036856"/>
+        <c:axId val="2083346344"/>
+        <c:axId val="2083351832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2074017096"/>
+        <c:axId val="2083346344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16195,14 +16142,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074036856"/>
+        <c:crossAx val="2083351832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16210,7 +16156,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074036856"/>
+        <c:axId val="2083351832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16233,14 +16179,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074017096"/>
+        <c:crossAx val="2083346344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -16250,7 +16195,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -16300,7 +16244,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -16661,11 +16604,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2074046936"/>
-        <c:axId val="-2074043832"/>
+        <c:axId val="2112847288"/>
+        <c:axId val="2112853112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2074046936"/>
+        <c:axId val="2112847288"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -16693,19 +16636,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074043832"/>
+        <c:crossAx val="2112853112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2074043832"/>
+        <c:axId val="2112853112"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -16729,21 +16671,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074046936"/>
+        <c:crossAx val="2112847288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -17217,11 +17157,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2074072920"/>
-        <c:axId val="-2074077848"/>
+        <c:axId val="2111919752"/>
+        <c:axId val="2111913928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2074072920"/>
+        <c:axId val="2111919752"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -17249,19 +17189,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074077848"/>
+        <c:crossAx val="2111913928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2074077848"/>
+        <c:axId val="2111913928"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -17285,21 +17224,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074072920"/>
+        <c:crossAx val="2111919752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -17351,7 +17288,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -18081,11 +18017,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1788279576"/>
-        <c:axId val="1788285096"/>
+        <c:axId val="2087377384"/>
+        <c:axId val="2087382840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1788279576"/>
+        <c:axId val="2087377384"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -18108,19 +18044,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788285096"/>
+        <c:crossAx val="2087382840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1788285096"/>
+        <c:axId val="2087382840"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -18149,14 +18084,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788279576"/>
+        <c:crossAx val="2087377384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18167,7 +18101,6 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -18224,7 +18157,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -18733,11 +18665,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121636008"/>
-        <c:axId val="2121794648"/>
+        <c:axId val="2087426616"/>
+        <c:axId val="2087432328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121636008"/>
+        <c:axId val="2087426616"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -18760,19 +18692,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121794648"/>
+        <c:crossAx val="2087432328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121794648"/>
+        <c:axId val="2087432328"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -18796,21 +18727,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121636008"/>
+        <c:crossAx val="2087426616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -18867,7 +18796,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -19284,11 +19212,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121609496"/>
-        <c:axId val="2121896680"/>
+        <c:axId val="2069918936"/>
+        <c:axId val="2069913368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121609496"/>
+        <c:axId val="2069918936"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -19311,19 +19239,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121896680"/>
+        <c:crossAx val="2069913368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121896680"/>
+        <c:axId val="2069913368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19346,21 +19273,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121609496"/>
+        <c:crossAx val="2069918936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -19412,7 +19337,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -19775,11 +19699,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121685368"/>
-        <c:axId val="2121522056"/>
+        <c:axId val="2122464952"/>
+        <c:axId val="2122470456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121685368"/>
+        <c:axId val="2122464952"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -19802,19 +19726,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121522056"/>
+        <c:crossAx val="2122470456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121522056"/>
+        <c:axId val="2122470456"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -19843,14 +19766,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121685368"/>
+        <c:crossAx val="2122464952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -19861,7 +19783,6 @@
         <c:idx val="3"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -19918,7 +19839,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -20420,11 +20340,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1788497704"/>
-        <c:axId val="1788503400"/>
+        <c:axId val="2122518152"/>
+        <c:axId val="2122523848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1788497704"/>
+        <c:axId val="2122518152"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -20447,19 +20367,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788503400"/>
+        <c:crossAx val="2122523848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1788503400"/>
+        <c:axId val="2122523848"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -20488,14 +20407,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1788497704"/>
+        <c:crossAx val="2122518152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -20506,7 +20424,6 @@
         <c:idx val="3"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -20563,7 +20480,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -20871,11 +20787,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121923736"/>
-        <c:axId val="2121559992"/>
+        <c:axId val="2122561992"/>
+        <c:axId val="2122567464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121923736"/>
+        <c:axId val="2122561992"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -20898,19 +20814,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121559992"/>
+        <c:crossAx val="2122567464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121559992"/>
+        <c:axId val="2122567464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20933,14 +20848,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121923736"/>
+        <c:crossAx val="2122561992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -20953,7 +20867,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -26289,8 +26202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF145"/>
   <sheetViews>
-    <sheetView topLeftCell="C113" workbookViewId="0">
-      <selection activeCell="L152" sqref="L152"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I74" sqref="I74:I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -28886,7 +28799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Nearly done with this chapter
</commit_message>
<xml_diff>
--- a/latex/performance_content/scaling/ItascaScaling.xlsx
+++ b/latex/performance_content/scaling/ItascaScaling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28420" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26540" windowHeight="14920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Strong 4.096M nodes" sheetId="1" r:id="rId1"/>
@@ -290,7 +290,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="460">
+  <cellStyleXfs count="478">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -751,8 +751,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -766,9 +784,8 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="41" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="41" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="460">
+  <cellStyles count="478">
     <cellStyle name="Comma" xfId="40" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1006,6 +1023,15 @@
     <cellStyle name="Followed Hyperlink" xfId="455" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="457" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="459" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="461" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="463" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="465" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="467" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="469" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="471" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="473" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="475" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="477" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1227,6 +1253,15 @@
     <cellStyle name="Hyperlink" xfId="454" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="456" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="458" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="460" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="462" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="464" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="466" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="468" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="470" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="472" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="474" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="476" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="41" builtinId="5"/>
   </cellStyles>
@@ -1256,22 +1291,23 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000"/>
               <a:t>Strong Scaling of SpMV + MPI Communication on Itasca</a:t>
             </a:r>
             <a:br>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000"/>
             </a:br>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000"/>
               <a:t>N=4096000 grid points; IMPI (MPI_Alltoallv)</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1682,6 +1718,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1712,16 +1749,12 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Time</a:t>
+                  <a:t>Time (ms)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (ms)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -1739,12 +1772,23 @@
         <c:idx val="3"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -1790,6 +1834,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2200,6 +2245,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2240,6 +2286,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -2257,6 +2304,7 @@
         <c:idx val="1"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2313,6 +2361,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2756,6 +2805,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2791,6 +2841,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
@@ -2804,6 +2855,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2860,6 +2912,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3203,6 +3256,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3237,6 +3291,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
@@ -3256,6 +3311,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3323,6 +3379,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3624,6 +3681,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3664,6 +3722,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
@@ -3677,6 +3736,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3733,6 +3793,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4164,6 +4225,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4204,6 +4266,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -4221,6 +4284,7 @@
         <c:idx val="1"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4277,6 +4341,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4611,6 +4676,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4645,6 +4711,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
@@ -4664,6 +4731,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4715,6 +4783,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5358,6 +5427,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5398,6 +5468,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -5417,6 +5488,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5468,6 +5540,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5793,6 +5866,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5833,6 +5907,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
@@ -5846,6 +5921,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5897,6 +5973,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6340,6 +6417,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6375,6 +6453,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6394,6 +6473,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6446,6 +6526,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6789,6 +6870,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6829,6 +6911,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6848,6 +6931,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6883,27 +6967,23 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Speedup</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of SpMV + MPI Communication on Itasca</a:t>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>Speedup of SpMV + MPI Communication on Itasca</a:t>
             </a:r>
             <a:br>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2000"/>
             </a:br>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2000"/>
               <a:t>N=4096000 grid points; IMPI (MPI_Alltoallv) </a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7417,6 +7497,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -7452,6 +7533,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -7469,12 +7551,23 @@
         <c:idx val="0"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -7520,6 +7613,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7863,6 +7957,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -7903,6 +7998,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -7922,6 +8018,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7957,21 +8054,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Weak Scaling</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of SpMV + MPI Communication on Itasca </a:t>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>Weak Scaling of SpMV + MPI on Itasca </a:t>
             </a:r>
             <a:br>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2000"/>
             </a:br>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2000"/>
               <a:t>Np = 4000 points, regular grid; IMPI (MPI_Alltoallv)</a:t>
             </a:r>
           </a:p>
@@ -8448,11 +8541,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Time</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (ms)</a:t>
+                  <a:t>Time (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -8478,6 +8567,16 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -8507,21 +8606,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Weak Scaling</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of SpMV (no MPI Communication) on Itasca </a:t>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>Weak Scaling of SpMV (no MPI Communication) on Itasca </a:t>
             </a:r>
             <a:br>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2000"/>
             </a:br>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2000"/>
               <a:t>Np = 4000 points regular grid</a:t>
             </a:r>
           </a:p>
@@ -8998,11 +9093,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Time</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (ms)</a:t>
+                  <a:t>Time (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -9028,6 +9119,16 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -9057,21 +9158,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Weak Scaling</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of MPI Communication (No SpMV) on Itasca </a:t>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>Weak Scaling of Communication Only on Itasca </a:t>
             </a:r>
             <a:br>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2000"/>
             </a:br>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2000"/>
               <a:t>Np = 4000 points; IMPI (MPI_Alltoallv)</a:t>
             </a:r>
           </a:p>
@@ -9516,11 +9613,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Time</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (ms)</a:t>
+                  <a:t>Time (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -9546,6 +9639,16 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -12411,6 +12514,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -12959,6 +13063,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -12994,6 +13099,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -13007,6 +13113,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13063,6 +13170,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -13406,6 +13514,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -13419,6 +13528,7 @@
       <c:valAx>
         <c:axId val="2087299368"/>
         <c:scaling>
+          <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -13440,6 +13550,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
@@ -13459,6 +13570,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13508,6 +13620,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -13966,6 +14079,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -14001,6 +14115,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -14014,6 +14129,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14063,6 +14179,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -14611,6 +14728,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -14646,6 +14764,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -14659,6 +14778,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14703,6 +14823,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -15131,6 +15252,7 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -15151,6 +15273,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
@@ -15164,6 +15287,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15553,6 +15677,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -15701,6 +15826,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -15735,6 +15861,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -15748,6 +15875,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15797,6 +15925,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -16142,6 +16271,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -16179,6 +16309,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -16195,6 +16326,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -16244,6 +16376,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -16636,6 +16769,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -16671,6 +16805,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -16684,6 +16819,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -17189,6 +17325,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -17224,6 +17361,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -17237,6 +17375,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -17272,22 +17411,23 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Strong Scaling of MPI Communication Only on Itasca</a:t>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>Strong Scaling of SpMV Only on Itasca</a:t>
             </a:r>
             <a:br>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000"/>
             </a:br>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>N=4096000 grid points; IMPI (MPI_Alltoallv)</a:t>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>N=4096000 grid points</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -17297,11 +17437,11 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Strong 4.096M nodes'!$B$6</c:f>
+              <c:f>'Strong 4.096M nodes'!$B$56</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -17390,367 +17530,6 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.187248</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Strong 4.096M nodes'!$C$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>n=31</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Strong 4.096M nodes'!$A$57:$A$67</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Strong 4.096M nodes'!$C$57:$C$67</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>229.491</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>102.828</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>71.77930000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>54.812</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>26.7995</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13.2852</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.62047</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.29734</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.65617</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.801324</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.330586</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Strong 4.096M nodes'!$D$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>n=50</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Strong 4.096M nodes'!$A$57:$A$67</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Strong 4.096M nodes'!$D$57:$D$67</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>338.264</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>161.435</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>121.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>85.3736</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>39.4875</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>19.6672</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.69557</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.78207</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.39753</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.2015</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.559307</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Strong 4.096M nodes'!$E$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>n=101 (NOT ENOUGH MEMORY)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Strong 4.096M nodes'!$A$57:$A$67</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Strong 4.096M nodes'!$E$57:$E$67</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Strong 4.096M nodes'!$B$105</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>n=17</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Strong 4.096M nodes'!$A$107:$A$116</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1024.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Strong 4.096M nodes'!$B$107:$B$116</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>15.2634</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18.9385</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.1997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.4392</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.670079999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.36441</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.05556</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.87821</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.3171</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.16531</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17762,7 +17541,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Strong 4.096M nodes'!$C$105</c:f>
+              <c:f>'Strong 4.096M nodes'!$C$56</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -17773,38 +17552,41 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Strong 4.096M nodes'!$A$107:$A$116</c:f>
+              <c:f>'Strong 4.096M nodes'!$A$57:$A$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>32.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>64.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>128.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>256.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>512.0</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>1024.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -17812,39 +17594,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Strong 4.096M nodes'!$C$107:$C$116</c:f>
+              <c:f>'Strong 4.096M nodes'!$C$57:$C$67</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>19.2692</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>229.491</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.1126</c:v>
+                  <c:v>102.828</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.0059</c:v>
+                  <c:v>71.77930000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.8831</c:v>
+                  <c:v>54.812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.93478</c:v>
+                  <c:v>26.7995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.14152</c:v>
+                  <c:v>13.2852</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.86099</c:v>
+                  <c:v>6.62047</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.92815</c:v>
+                  <c:v>3.29734</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8335</c:v>
+                  <c:v>1.65617</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.45715</c:v>
+                  <c:v>0.801324</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.330586</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17856,7 +17641,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Strong 4.096M nodes'!$D$105</c:f>
+              <c:f>'Strong 4.096M nodes'!$D$56</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -17867,38 +17652,41 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Strong 4.096M nodes'!$A$107:$A$116</c:f>
+              <c:f>'Strong 4.096M nodes'!$A$57:$A$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>32.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>64.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>128.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>256.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>512.0</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>1024.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -17906,104 +17694,43 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Strong 4.096M nodes'!$D$107:$D$116</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>32.4221</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>33.5358</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22.5202</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.3696</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.34446</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.93506</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.0301</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.46343</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.9892</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.44446</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Strong 4.096M nodes'!$E$105</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>n=101 (NOT ENOUGH MEMORY)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Strong 4.096M nodes'!$A$107:$A$116</c:f>
+              <c:f>'Strong 4.096M nodes'!$D$57:$D$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>338.264</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>161.435</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0</c:v>
+                  <c:v>121.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.0</c:v>
+                  <c:v>85.3736</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.0</c:v>
+                  <c:v>39.4875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>64.0</c:v>
+                  <c:v>19.6672</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>128.0</c:v>
+                  <c:v>9.69557</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>256.0</c:v>
+                  <c:v>4.78207</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>512.0</c:v>
+                  <c:v>2.39753</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1024.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Strong 4.096M nodes'!$E$107:$E$116</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                  <c:v>1.2015</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.559307</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -18044,6 +17771,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -18074,16 +17802,12 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Time</a:t>
+                  <a:t>Time (ms)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (ms)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -18097,16 +17821,23 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:legendEntry>
-        <c:idx val="7"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -18157,6 +17888,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -18692,6 +18424,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -18727,6 +18460,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
@@ -18740,6 +18474,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -18796,6 +18531,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -19239,6 +18975,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -19252,6 +18989,7 @@
       <c:valAx>
         <c:axId val="2069913368"/>
         <c:scaling>
+          <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -19273,6 +19011,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
@@ -19286,6 +19025,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -19321,22 +19061,23 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000"/>
               <a:t>Strong Scaling of MPI Communication Only on Itasca</a:t>
             </a:r>
             <a:br>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000"/>
             </a:br>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000"/>
               <a:t>N=4096000 grid points; IMPI (MPI_Alltoallv)</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -19726,6 +19467,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -19756,16 +19498,12 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Time</a:t>
+                  <a:t>Time (ms)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (ms)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
@@ -19783,12 +19521,23 @@
         <c:idx val="3"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -19839,6 +19588,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -20367,6 +20117,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -20407,6 +20158,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -20424,6 +20176,7 @@
         <c:idx val="3"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -20480,6 +20233,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -20814,6 +20568,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -20848,6 +20603,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
@@ -20867,6 +20623,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -20924,7 +20681,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -21528,16 +21285,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>92364</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>168564</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22410,8 +22167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X305"/>
   <sheetViews>
-    <sheetView topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="H189" sqref="H189"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -26202,8 +25959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="I74" sqref="I74:I84"/>
+    <sheetView topLeftCell="L57" workbookViewId="0">
+      <selection activeCell="K67" sqref="K67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -26269,6 +26026,10 @@
       <c r="H4" s="1">
         <v>0.10539999999999999</v>
       </c>
+      <c r="I4">
+        <f>H4/H4</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:32">
       <c r="A5">
@@ -26295,6 +26056,10 @@
       <c r="H5" s="1">
         <v>0.1082</v>
       </c>
+      <c r="I5">
+        <f>$H$4/$H5</f>
+        <v>0.97412199630314222</v>
+      </c>
     </row>
     <row r="6" spans="1:32">
       <c r="A6">
@@ -26321,6 +26086,10 @@
       <c r="H6" s="1">
         <v>0.11045000000000001</v>
       </c>
+      <c r="I6">
+        <f>$H$4/$H6</f>
+        <v>0.95427795382526015</v>
+      </c>
     </row>
     <row r="7" spans="1:32">
       <c r="A7">
@@ -26347,6 +26116,10 @@
       <c r="H7" s="1">
         <v>0.26788800000000001</v>
       </c>
+      <c r="I7">
+        <f>$H$4/$H7</f>
+        <v>0.39344800812279757</v>
+      </c>
     </row>
     <row r="8" spans="1:32">
       <c r="A8">
@@ -26373,6 +26146,10 @@
       <c r="H8" s="1">
         <v>0.33501900000000001</v>
       </c>
+      <c r="I8">
+        <f>$H$4/$H8</f>
+        <v>0.3146090221748617</v>
+      </c>
     </row>
     <row r="9" spans="1:32">
       <c r="A9">
@@ -26399,6 +26176,10 @@
       <c r="H9" s="1">
         <v>0.40115000000000001</v>
       </c>
+      <c r="I9">
+        <f>$H$4/$H9</f>
+        <v>0.26274460924841081</v>
+      </c>
     </row>
     <row r="10" spans="1:32">
       <c r="A10">
@@ -26425,6 +26206,10 @@
       <c r="H10">
         <v>0.451181</v>
       </c>
+      <c r="I10">
+        <f>$H$4/$H10</f>
+        <v>0.23360912804395573</v>
+      </c>
     </row>
     <row r="11" spans="1:32">
       <c r="A11">
@@ -26451,6 +26236,10 @@
       <c r="H11">
         <v>0.67816399999999999</v>
       </c>
+      <c r="I11">
+        <f>$H$4/$H11</f>
+        <v>0.15541963300912462</v>
+      </c>
     </row>
     <row r="12" spans="1:32">
       <c r="A12">
@@ -26477,6 +26266,10 @@
       <c r="H12">
         <v>0.80666099999999996</v>
       </c>
+      <c r="I12">
+        <f>$H$4/$H12</f>
+        <v>0.13066207489887324</v>
+      </c>
     </row>
     <row r="13" spans="1:32">
       <c r="A13">
@@ -26503,6 +26296,10 @@
       <c r="H13">
         <v>1.1890400000000001</v>
       </c>
+      <c r="I13">
+        <f>$H$4/$H13</f>
+        <v>8.8642938841418273E-2</v>
+      </c>
       <c r="AF13" t="s">
         <v>52</v>
       </c>
@@ -26529,7 +26326,10 @@
       <c r="H14" s="1">
         <v>1.6982299999999999</v>
       </c>
-      <c r="I14" s="11"/>
+      <c r="I14">
+        <f>$H$4/$H14</f>
+        <v>6.206462022223138E-2</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35">
@@ -27983,8 +27783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Found another old poster. could include the data but I would have to update the code and test again
</commit_message>
<xml_diff>
--- a/latex/performance_content/scaling/ItascaScaling.xlsx
+++ b/latex/performance_content/scaling/ItascaScaling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26540" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26540" windowHeight="14920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Strong 4.096M nodes" sheetId="1" r:id="rId1"/>
@@ -22167,7 +22167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
@@ -25959,8 +25959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF145"/>
   <sheetViews>
-    <sheetView topLeftCell="L57" workbookViewId="0">
-      <selection activeCell="K67" sqref="K67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -26329,6 +26329,12 @@
       <c r="I14">
         <f>$H$4/$H14</f>
         <v>6.206462022223138E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="D23" s="1">
+        <f>D8/D9</f>
+        <v>0.80954735168083858</v>
       </c>
     </row>
     <row r="35" spans="1:8">

</xml_diff>